<commit_message>
R analysis modified. Using MEDIAN
</commit_message>
<xml_diff>
--- a/Analysis/Excel/SummaryPerUser.xlsx
+++ b/Analysis/Excel/SummaryPerUser.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="295">
   <si>
     <t xml:space="preserve">Obs: Dados referentes as ações realizadas somente no tempo trabalhado</t>
   </si>
@@ -700,6 +700,12 @@
   </si>
   <si>
     <t xml:space="preserve">Leve dor no pulso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">only tasks 3 and 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all tasks</t>
   </si>
   <si>
     <t xml:space="preserve">team1</t>
@@ -1033,28 +1039,23 @@
   </sheetPr>
   <dimension ref="A1:BU213"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B140" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B58" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A140" activeCellId="0" sqref="A140"/>
-      <selection pane="bottomRight" activeCell="W212" activeCellId="0" sqref="W212"/>
+      <selection pane="bottomLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
+      <selection pane="bottomRight" activeCell="P115" activeCellId="0" sqref="P115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.53571428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="9" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="17" min="15" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="22" min="19" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="73" min="24" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="74" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="73" min="24" style="0" width="24.9744897959184"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="85.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2092,7 +2093,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
         <v>5</v>
       </c>
@@ -2301,7 +2302,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
         <v>5</v>
       </c>
@@ -2519,7 +2520,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
         <v>6</v>
       </c>
@@ -2740,7 +2741,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="n">
         <v>6</v>
       </c>
@@ -2961,7 +2962,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="n">
         <v>13</v>
       </c>
@@ -3158,7 +3159,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="n">
         <v>13</v>
       </c>
@@ -3358,7 +3359,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="n">
         <v>22</v>
       </c>
@@ -3549,7 +3550,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="n">
         <v>22</v>
       </c>
@@ -12176,21 +12177,53 @@
         <v>0.136363636363636</v>
       </c>
     </row>
+    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C62" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="I62" s="0" t="s">
+        <v>227</v>
+      </c>
+    </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C63" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="F63" s="0" t="s">
+        <v>231</v>
+      </c>
       <c r="I63" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="J63" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K63" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="L63" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C64" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="E64" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="F64" s="0" t="n">
+        <v>18</v>
+      </c>
       <c r="I64" s="0" t="n">
         <v>10</v>
       </c>
@@ -12205,6 +12238,18 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C65" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="F65" s="0" t="n">
+        <v>13</v>
+      </c>
       <c r="I65" s="0" t="n">
         <v>16</v>
       </c>
@@ -12219,6 +12264,18 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C66" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="E66" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="F66" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="I66" s="0" t="n">
         <v>6</v>
       </c>
@@ -12233,6 +12290,18 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C67" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="E67" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="F67" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="I67" s="0" t="n">
         <v>10</v>
       </c>
@@ -12247,6 +12316,18 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C68" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="D68" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="E68" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="F68" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="I68" s="0" t="n">
         <v>7</v>
       </c>
@@ -12261,6 +12342,18 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C69" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="E69" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F69" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="I69" s="0" t="n">
         <v>10</v>
       </c>
@@ -12275,6 +12368,18 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C70" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="F70" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="I70" s="0" t="n">
         <v>6</v>
       </c>
@@ -12289,6 +12394,18 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C71" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="D71" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="E71" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F71" s="0" t="n">
+        <v>8</v>
+      </c>
       <c r="I71" s="0" t="n">
         <v>10</v>
       </c>
@@ -12303,6 +12420,18 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C72" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="D72" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="E72" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="F72" s="0" t="n">
+        <v>14</v>
+      </c>
       <c r="I72" s="0" t="n">
         <v>12</v>
       </c>
@@ -12317,6 +12446,18 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C73" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="E73" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="F73" s="0" t="n">
+        <v>11</v>
+      </c>
       <c r="I73" s="0" t="n">
         <v>9</v>
       </c>
@@ -12331,6 +12472,15 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D74" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="E74" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="F74" s="0" t="n">
+        <v>17</v>
+      </c>
       <c r="I74" s="0" t="n">
         <v>21</v>
       </c>
@@ -12345,6 +12495,15 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D75" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="E75" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F75" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="I75" s="0" t="n">
         <v>24</v>
       </c>
@@ -12359,6 +12518,15 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D76" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="E76" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="F76" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="I76" s="0" t="n">
         <v>32</v>
       </c>
@@ -12373,6 +12541,15 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D77" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="E77" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="F77" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="I77" s="0" t="n">
         <v>49</v>
       </c>
@@ -12387,6 +12564,15 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D78" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="E78" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F78" s="0" t="n">
+        <v>15</v>
+      </c>
       <c r="I78" s="0" t="n">
         <v>19</v>
       </c>
@@ -12400,10 +12586,19 @@
         <v>3</v>
       </c>
       <c r="O78" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D79" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="E79" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F79" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="I79" s="0" t="n">
         <v>21</v>
       </c>
@@ -12417,13 +12612,19 @@
         <v>22</v>
       </c>
       <c r="N79" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="O79" s="0" t="n">
         <v>44.0515</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E80" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F80" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="I80" s="0" t="n">
         <v>23</v>
       </c>
@@ -12437,13 +12638,19 @@
         <v>1</v>
       </c>
       <c r="N80" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="O80" s="0" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E81" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F81" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="I81" s="0" t="n">
         <v>21</v>
       </c>
@@ -12457,13 +12664,19 @@
         <v>1</v>
       </c>
       <c r="N81" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="O81" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E82" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="F82" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="I82" s="0" t="n">
         <v>45</v>
       </c>
@@ -12477,13 +12690,19 @@
         <v>1</v>
       </c>
       <c r="N82" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="O82" s="0" t="n">
         <v>3297.5</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E83" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="F83" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="I83" s="0" t="n">
         <v>33</v>
       </c>
@@ -12497,13 +12716,19 @@
         <v>0</v>
       </c>
       <c r="N83" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="O83" s="0" t="n">
         <v>4313</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E84" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="F84" s="0" t="n">
+        <v>9</v>
+      </c>
       <c r="J84" s="0" t="n">
         <v>14</v>
       </c>
@@ -12514,13 +12739,19 @@
         <v>1</v>
       </c>
       <c r="N84" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="O84" s="0" t="n">
         <v>6794.5</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E85" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="F85" s="0" t="n">
+        <v>15</v>
+      </c>
       <c r="J85" s="0" t="n">
         <v>19</v>
       </c>
@@ -12531,13 +12762,19 @@
         <v>2</v>
       </c>
       <c r="N85" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="O85" s="0" t="n">
         <v>6505</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E86" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="F86" s="0" t="n">
+        <v>20</v>
+      </c>
       <c r="J86" s="0" t="n">
         <v>41</v>
       </c>
@@ -12548,13 +12785,19 @@
         <v>3</v>
       </c>
       <c r="N86" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="O86" s="0" t="n">
         <v>164.875</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E87" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F87" s="0" t="n">
+        <v>11</v>
+      </c>
       <c r="J87" s="0" t="n">
         <v>11</v>
       </c>
@@ -12565,13 +12808,19 @@
         <v>1</v>
       </c>
       <c r="N87" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="O87" s="0" t="n">
         <v>134.7813</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E88" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="F88" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="J88" s="0" t="n">
         <v>17</v>
       </c>
@@ -12582,13 +12831,19 @@
         <v>2</v>
       </c>
       <c r="N88" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="O88" s="0" t="n">
         <v>94.3681</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E89" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F89" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="J89" s="0" t="n">
         <v>29</v>
       </c>
@@ -12599,13 +12854,19 @@
         <v>1</v>
       </c>
       <c r="N89" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="O89" s="0" t="n">
         <v>81.3125</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E90" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="F90" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="J90" s="0" t="n">
         <v>11</v>
       </c>
@@ -12617,6 +12878,12 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E91" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="F91" s="0" t="n">
+        <v>10</v>
+      </c>
       <c r="J91" s="0" t="n">
         <v>38</v>
       </c>
@@ -12627,22 +12894,28 @@
         <v>3</v>
       </c>
       <c r="N91" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="O91" s="0" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="P91" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="Q91" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="R91" s="0" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E92" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="F92" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="J92" s="0" t="n">
         <v>9</v>
       </c>
@@ -12653,7 +12926,7 @@
         <v>1</v>
       </c>
       <c r="N92" s="0" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="O92" s="0" t="n">
         <v>30.0938</v>
@@ -12665,10 +12938,16 @@
         <v>2.635</v>
       </c>
       <c r="R92" s="0" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E93" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F93" s="0" t="n">
+        <v>23</v>
+      </c>
       <c r="J93" s="0" t="n">
         <v>14</v>
       </c>
@@ -12679,7 +12958,7 @@
         <v>4</v>
       </c>
       <c r="N93" s="0" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="O93" s="0" t="n">
         <v>70.5069</v>
@@ -12691,10 +12970,16 @@
         <v>2.635</v>
       </c>
       <c r="R93" s="0" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E94" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="F94" s="0" t="n">
+        <v>22</v>
+      </c>
       <c r="J94" s="0" t="n">
         <v>37</v>
       </c>
@@ -12705,7 +12990,7 @@
         <v>4</v>
       </c>
       <c r="N94" s="0" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="O94" s="0" t="n">
         <v>83.5625</v>
@@ -12717,10 +13002,16 @@
         <v>2.635</v>
       </c>
       <c r="R94" s="0" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E95" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="F95" s="0" t="n">
+        <v>9</v>
+      </c>
       <c r="J95" s="0" t="n">
         <v>19</v>
       </c>
@@ -12731,7 +13022,7 @@
         <v>2</v>
       </c>
       <c r="N95" s="0" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="O95" s="0" t="n">
         <v>40.4132</v>
@@ -12743,10 +13034,16 @@
         <v>2.635</v>
       </c>
       <c r="R95" s="0" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E96" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F96" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K96" s="0" t="n">
         <v>1</v>
       </c>
@@ -12754,7 +13051,7 @@
         <v>1</v>
       </c>
       <c r="N96" s="0" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="O96" s="0" t="n">
         <v>53.4688</v>
@@ -12766,10 +13063,16 @@
         <v>2.635</v>
       </c>
       <c r="R96" s="0" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E97" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F97" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K97" s="0" t="n">
         <v>15</v>
       </c>
@@ -12777,7 +13080,7 @@
         <v>8</v>
       </c>
       <c r="N97" s="0" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="O97" s="0" t="n">
         <v>13.0556</v>
@@ -12789,10 +13092,16 @@
         <v>2.635</v>
       </c>
       <c r="R97" s="0" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E98" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="F98" s="0" t="n">
+        <v>10</v>
+      </c>
       <c r="K98" s="0" t="n">
         <v>6</v>
       </c>
@@ -12801,6 +13110,12 @@
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E99" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F99" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K99" s="0" t="n">
         <v>6</v>
       </c>
@@ -12809,6 +13124,9 @@
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F100" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K100" s="0" t="n">
         <v>8</v>
       </c>
@@ -12817,6 +13135,9 @@
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F101" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="K101" s="0" t="n">
         <v>34</v>
       </c>
@@ -12825,6 +13146,9 @@
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F102" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="K102" s="0" t="n">
         <v>19</v>
       </c>
@@ -12833,6 +13157,9 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F103" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K103" s="0" t="n">
         <v>18</v>
       </c>
@@ -12912,7 +13239,7 @@
         <v>14</v>
       </c>
       <c r="U112" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="V112" s="0" t="n">
         <v>1</v>
@@ -14114,7 +14441,7 @@
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U163" s="0" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="V163" s="0" t="n">
         <v>1</v>
@@ -15176,13 +15503,13 @@
   </sheetPr>
   <dimension ref="A1:BP9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="4" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="4" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15290,7 +15617,7 @@
         <v>3</v>
       </c>
       <c r="AK1" s="5" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="AL1" s="5" t="n">
         <v>5</v>
@@ -15312,7 +15639,7 @@
         <v>3</v>
       </c>
       <c r="AS1" s="5" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="AT1" s="5" t="n">
         <v>2</v>
@@ -15328,34 +15655,34 @@
         <v>4</v>
       </c>
       <c r="AY1" s="5" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="AZ1" s="5" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="BA1" s="5" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="BB1" s="5" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="BC1" s="5" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="BD1" s="5" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="BE1" s="5" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="BF1" s="5" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="BG1" s="5" t="n">
         <v>4</v>
       </c>
       <c r="BH1" s="5" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="BI1" s="5" t="s">
         <v>83</v>
@@ -15511,28 +15838,28 @@
         <v>4</v>
       </c>
       <c r="AY2" s="5" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="AZ2" s="5" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="BA2" s="5" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="BB2" s="5" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="BC2" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="BD2" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="BE2" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="BD2" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="BE2" s="5" t="s">
-        <v>261</v>
-      </c>
       <c r="BF2" s="5" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="BG2" s="5" t="n">
         <v>4</v>
@@ -15648,7 +15975,7 @@
         <v>5</v>
       </c>
       <c r="AG3" s="5" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="AH3" s="5" t="n">
         <v>5</v>
@@ -15687,7 +16014,7 @@
         <v>5</v>
       </c>
       <c r="AV3" s="5" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="AW3" s="5" t="n">
         <v>5</v>
@@ -15734,7 +16061,7 @@
       </c>
       <c r="BL3" s="0"/>
       <c r="BM3" s="5" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="BN3" s="5" t="s">
         <v>83</v>
@@ -15841,7 +16168,7 @@
         <v>3</v>
       </c>
       <c r="AG4" s="5" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="AH4" s="5" t="n">
         <v>5</v>
@@ -15853,7 +16180,7 @@
         <v>5</v>
       </c>
       <c r="AK4" s="5" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="AL4" s="5" t="n">
         <v>5</v>
@@ -15865,7 +16192,7 @@
         <v>5</v>
       </c>
       <c r="AO4" s="5" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="AP4" s="5" t="n">
         <v>5</v>
@@ -15877,7 +16204,7 @@
         <v>4</v>
       </c>
       <c r="AS4" s="5" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="AT4" s="5" t="n">
         <v>3</v>
@@ -15886,7 +16213,7 @@
         <v>5</v>
       </c>
       <c r="AV4" s="5" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="AW4" s="5" t="n">
         <v>4</v>
@@ -15922,7 +16249,7 @@
         <v>4</v>
       </c>
       <c r="BH4" s="5" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="BI4" s="5" t="s">
         <v>76</v>
@@ -15935,7 +16262,7 @@
       </c>
       <c r="BL4" s="0"/>
       <c r="BM4" s="5" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="BN4" s="5" t="s">
         <v>83</v>
@@ -16111,7 +16438,7 @@
       </c>
       <c r="BG5" s="0"/>
       <c r="BH5" s="5" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="BI5" s="5" t="s">
         <v>83</v>
@@ -16266,7 +16593,7 @@
         <v>5</v>
       </c>
       <c r="AV6" s="5" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="AW6" s="5" t="n">
         <v>5</v>
@@ -16300,7 +16627,7 @@
       </c>
       <c r="BG6" s="0"/>
       <c r="BH6" s="5" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="BI6" s="5" t="s">
         <v>83</v>
@@ -16460,34 +16787,34 @@
         <v>4</v>
       </c>
       <c r="AY7" s="5" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="AZ7" s="5" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="BA7" s="5" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="BB7" s="5" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="BC7" s="5" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="BD7" s="5" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="BE7" s="5" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="BF7" s="5" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="BG7" s="5" t="n">
         <v>4</v>
       </c>
       <c r="BH7" s="5" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="BI7" s="5" t="s">
         <v>83</v>
@@ -16499,7 +16826,7 @@
         <v>83</v>
       </c>
       <c r="BL7" s="5" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="BM7" s="0"/>
       <c r="BN7" s="0"/>
@@ -16611,7 +16938,7 @@
         <v>4</v>
       </c>
       <c r="AK8" s="5" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="AL8" s="5" t="n">
         <v>5</v>
@@ -16633,7 +16960,7 @@
         <v>4</v>
       </c>
       <c r="AS8" s="5" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="AT8" s="5" t="n">
         <v>3</v>
@@ -16649,34 +16976,34 @@
         <v>5</v>
       </c>
       <c r="AY8" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="AZ8" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="BA8" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="AZ8" s="5" t="s">
+      <c r="BB8" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="BC8" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="BD8" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="BE8" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="BA8" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="BB8" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="BC8" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="BD8" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="BE8" s="5" t="s">
-        <v>261</v>
-      </c>
       <c r="BF8" s="5" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="BG8" s="5" t="n">
         <v>5</v>
       </c>
       <c r="BH8" s="5" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="BI8" s="5" t="s">
         <v>76</v>
@@ -16688,7 +17015,7 @@
         <v>76</v>
       </c>
       <c r="BL8" s="5" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="BM8" s="0"/>
       <c r="BN8" s="0"/>
@@ -16790,7 +17117,7 @@
         <v>5</v>
       </c>
       <c r="AG9" s="5" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="AH9" s="5" t="n">
         <v>4</v>
@@ -16802,7 +17129,7 @@
         <v>4</v>
       </c>
       <c r="AK9" s="5" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="AL9" s="5" t="n">
         <v>5</v>
@@ -16814,7 +17141,7 @@
         <v>5</v>
       </c>
       <c r="AO9" s="5" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="AP9" s="5" t="n">
         <v>4</v>
@@ -16826,7 +17153,7 @@
         <v>4</v>
       </c>
       <c r="AS9" s="5" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="AT9" s="5" t="n">
         <v>2</v>
@@ -16835,7 +17162,7 @@
         <v>5</v>
       </c>
       <c r="AV9" s="5" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="AW9" s="5" t="n">
         <v>4</v>
@@ -16844,34 +17171,34 @@
         <v>5</v>
       </c>
       <c r="AY9" s="5" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="AZ9" s="5" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="BA9" s="5" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="BB9" s="5" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="BC9" s="5" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="BD9" s="5" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="BE9" s="5" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="BF9" s="5" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="BG9" s="5" t="n">
         <v>4</v>
       </c>
       <c r="BH9" s="5" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="BI9" s="5" t="s">
         <v>83</v>
@@ -16883,10 +17210,10 @@
         <v>83</v>
       </c>
       <c r="BL9" s="5" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="BM9" s="5" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="BN9" s="5"/>
       <c r="BO9" s="5"/>
@@ -16910,20 +17237,23 @@
   </sheetPr>
   <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>